<commit_message>
created organization rest endpoints
</commit_message>
<xml_diff>
--- a/doc/api-mapping.xlsx
+++ b/doc/api-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\easysix\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F095B8-83F4-4327-A2BB-2D1096B8FE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED30E00B-551B-4A7E-9FAF-8912646508AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4D5A77EA-79A3-4D58-8216-51A32A05CB26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{4D5A77EA-79A3-4D58-8216-51A32A05CB26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,12 +134,6 @@
     <t>DomainObject</t>
   </si>
   <si>
-    <t>/host/[name]</t>
-  </si>
-  <si>
-    <t>/domain/[name]</t>
-  </si>
-  <si>
     <t>HostObject</t>
   </si>
   <si>
@@ -149,18 +143,9 @@
     <t>AuthInfo</t>
   </si>
   <si>
-    <t>/domain/transfer/[name]</t>
-  </si>
-  <si>
-    <t>/domain/renew/[name]</t>
-  </si>
-  <si>
     <t>RenewPeriod</t>
   </si>
   <si>
-    <t>/domain/querytransfer/[name]</t>
-  </si>
-  <si>
     <t>ORGANIZATIONINFO</t>
   </si>
   <si>
@@ -180,6 +165,21 @@
   </si>
   <si>
     <t>/organization/[id]</t>
+  </si>
+  <si>
+    <t>/domain/[id]</t>
+  </si>
+  <si>
+    <t>/domain/transfer/[id]</t>
+  </si>
+  <si>
+    <t>/domain/renew/[id]</t>
+  </si>
+  <si>
+    <t>/domain/querytransfer/[id]</t>
+  </si>
+  <si>
+    <t>/host/[id]</t>
   </si>
 </sst>
 </file>
@@ -563,21 +563,21 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -592,7 +592,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -606,7 +606,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -620,7 +620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -628,13 +628,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -645,7 +645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -659,7 +659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -667,13 +667,13 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -681,13 +681,13 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -695,10 +695,10 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -706,10 +706,10 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -717,13 +717,13 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -731,13 +731,13 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -745,13 +745,13 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -762,10 +762,10 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -773,13 +773,13 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -790,10 +790,10 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -801,10 +801,10 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -815,57 +815,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>